<commit_message>
The product page is half done
</commit_message>
<xml_diff>
--- a/documents/заполнение бд/categories.xlsx
+++ b/documents/заполнение бд/categories.xlsx
@@ -24,34 +24,34 @@
     <t>title</t>
   </si>
   <si>
-    <t>Электроника</t>
-  </si>
-  <si>
-    <t>Косметика и парфюмерия</t>
-  </si>
-  <si>
     <t>Аксессуары</t>
   </si>
   <si>
-    <t>Домашний декор</t>
-  </si>
-  <si>
     <t>Одежда</t>
   </si>
   <si>
-    <t>Кулинарные наборы</t>
-  </si>
-  <si>
-    <t>Спортивные товары</t>
-  </si>
-  <si>
-    <t>Настольные игры и пазлы</t>
-  </si>
-  <si>
     <t>Книги</t>
   </si>
   <si>
-    <t>Товары для хобби и творчества</t>
+    <t>Декор</t>
+  </si>
+  <si>
+    <t>Косметика</t>
+  </si>
+  <si>
+    <t>Кулинария</t>
+  </si>
+  <si>
+    <t>Игры</t>
+  </si>
+  <si>
+    <t>Спорт</t>
+  </si>
+  <si>
+    <t>Хобби</t>
+  </si>
+  <si>
+    <t>Гаджеты</t>
   </si>
 </sst>
 </file>
@@ -372,7 +372,7 @@
   <dimension ref="A1:A11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -392,7 +392,7 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
@@ -402,22 +402,22 @@
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.3">
@@ -436,6 +436,9 @@
       </c>
     </row>
   </sheetData>
+  <sortState ref="A2:A11">
+    <sortCondition ref="A11"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>